<commit_message>
fix heights of title text boxes to match wrapped text
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Id</t>
   </si>
@@ -31,7 +31,7 @@
     <t>Created</t>
   </si>
   <si>
-    <t>line wrap long descriptions and increase textbox height to accomodate</t>
+    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
   </si>
   <si>
     <t>Todo</t>
@@ -40,23 +40,14 @@
     <t>Bug</t>
   </si>
   <si>
-    <t>10/27/2017</t>
-  </si>
-  <si>
-    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
-  </si>
-  <si>
     <t>10/28/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">program icon </t>
-  </si>
-  <si>
-    <t>Feature</t>
   </si>
   <si>
     <t xml:space="preserve">have some key command to end the current task
 and immediately open and edit a new task below it</t>
+  </si>
+  <si>
+    <t>Feature</t>
   </si>
   <si>
     <t>12/1/2017</t>
@@ -140,6 +131,21 @@
     <t>Done</t>
   </si>
   <si>
+    <t>line wrap long descriptions and increase textbox height to accomodate</t>
+  </si>
+  <si>
+    <t>10/27/2017</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">program icon </t>
+  </si>
+  <si>
+    <t>2/26/2018</t>
+  </si>
+  <si>
     <t>Active</t>
   </si>
   <si>
@@ -156,9 +162,6 @@
   </si>
   <si>
     <t>Skip</t>
-  </si>
-  <si>
-    <t>2/26/2018</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -237,7 +240,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -254,7 +257,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -263,282 +266,265 @@
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0">
-        <v>19</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -548,7 +534,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -571,27 +557,47 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>45</v>
+      <c r="B3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -612,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -620,7 +626,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
@@ -628,10 +634,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0">
         <v>20</v>
@@ -639,21 +645,21 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
@@ -661,10 +667,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
turn textbox resizing back on
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>Id</t>
   </si>
@@ -31,13 +31,25 @@
     <t>Created</t>
   </si>
   <si>
+    <t>Have executable be named Tamax.exe to match installation program name</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
+  </si>
+  <si>
+    <t>get the msi installed program to run again - it won't run</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
     <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
-  </si>
-  <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Bug</t>
   </si>
   <si>
     <t>10/28/2017</t>
@@ -45,9 +57,6 @@
   <si>
     <t xml:space="preserve">have some key command to end the current task
 and immediately open and edit a new task below it</t>
-  </si>
-  <si>
-    <t>Feature</t>
   </si>
   <si>
     <t>12/1/2017</t>
@@ -135,9 +144,6 @@
   </si>
   <si>
     <t>10/27/2017</t>
-  </si>
-  <si>
-    <t>3/2/2018</t>
   </si>
   <si>
     <t xml:space="preserve">program icon </t>
@@ -214,7 +220,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -240,7 +246,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -257,7 +263,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -269,29 +275,29 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
@@ -300,52 +306,52 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -354,29 +360,29 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>19</v>
@@ -385,83 +391,83 @@
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>28</v>
@@ -473,29 +479,29 @@
         <v>10</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>31</v>
@@ -504,27 +510,61 @@
         <v>6</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0">
         <v>19</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>34</v>
+      <c r="B20" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -557,7 +597,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2">
@@ -565,19 +605,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -585,19 +625,19 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -618,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -626,7 +666,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2">
@@ -634,43 +674,43 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="D3" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renaming project to Tamarin
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Id</t>
   </si>
@@ -31,22 +31,16 @@
     <t>Created</t>
   </si>
   <si>
-    <t>Have executable be named Tamax.exe to match installation program name</t>
+    <t>get the msi installed program to run again - it won't run</t>
   </si>
   <si>
     <t>Todo</t>
   </si>
   <si>
-    <t>Feature</t>
+    <t>Bug</t>
   </si>
   <si>
     <t>3/2/2018</t>
-  </si>
-  <si>
-    <t>get the msi installed program to run again - it won't run</t>
-  </si>
-  <si>
-    <t>Bug</t>
   </si>
   <si>
     <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
@@ -57,6 +51,9 @@
   <si>
     <t xml:space="preserve">have some key command to end the current task
 and immediately open and edit a new task below it</t>
+  </si>
+  <si>
+    <t>Feature</t>
   </si>
   <si>
     <t>12/1/2017</t>
@@ -138,6 +135,13 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have executable be named Tamarin.exe to match installation program name
+-update installer to Tamarin</t>
+  </si>
+  <si>
+    <t>3/3/2018</t>
   </si>
   <si>
     <t>line wrap long descriptions and increase textbox height to accomodate</t>
@@ -220,7 +224,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -246,7 +250,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -263,7 +267,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -272,15 +276,15 @@
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -289,32 +293,32 @@
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>15</v>
@@ -323,15 +327,15 @@
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>16</v>
@@ -340,15 +344,15 @@
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>17</v>
@@ -357,15 +361,15 @@
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>18</v>
@@ -377,12 +381,12 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>19</v>
@@ -391,18 +395,18 @@
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -411,49 +415,49 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -462,29 +466,29 @@
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>30</v>
@@ -493,15 +497,15 @@
         <v>6</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>31</v>
@@ -510,61 +514,44 @@
         <v>6</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="0">
-        <v>19</v>
-      </c>
-      <c r="B20" s="0" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -574,7 +561,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -597,47 +584,67 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="0" t="s">
+      <c r="B4" s="0" t="s">
         <v>42</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -658,7 +665,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -666,7 +673,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2">
@@ -674,10 +681,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0">
         <v>22</v>
@@ -685,32 +692,32 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>48</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ctrl-N to open new next task
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -31,40 +31,24 @@
     <t>Created</t>
   </si>
   <si>
-    <t>get the msi installed program to run again - it won't run</t>
-  </si>
-  <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>3/2/2018</t>
-  </si>
-  <si>
-    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
-  </si>
-  <si>
-    <t>10/28/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">have some key command to end the current task
-and immediately open and edit a new task below it</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>12/1/2017</t>
-  </si>
-  <si>
     <t xml:space="preserve">if category A is removed, and category B is added,
 and category A is a starting-sub-string of B
 then all category A tasks are auto reset to B - they should not be</t>
   </si>
   <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>12/1/2017</t>
+  </si>
+  <si>
     <t>tabbing from text should move to next text, not the drop downs</t>
+  </si>
+  <si>
+    <t>Feature</t>
   </si>
   <si>
     <t>down-arrow from last line of text should move into next text box</t>
@@ -134,14 +118,31 @@
     <t>1/7/2018</t>
   </si>
   <si>
+    <t>get the msi installed program to run again - it won't run</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
+  </si>
+  <si>
+    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
+  </si>
+  <si>
+    <t>10/28/2017</t>
+  </si>
+  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">have some key command to end the current task
+and immediately open and edit a new task below it
+Ctrl-N (Next or New)</t>
+  </si>
+  <si>
+    <t>3/3/2018</t>
   </si>
   <si>
     <t xml:space="preserve">Have executable be named Tamarin.exe to match installation program name
 -update installer to Tamarin</t>
-  </si>
-  <si>
-    <t>3/3/2018</t>
   </si>
   <si>
     <t>line wrap long descriptions and increase textbox height to accomodate</t>
@@ -224,7 +225,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -250,7 +251,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -267,7 +268,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -276,15 +277,15 @@
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -293,83 +294,83 @@
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>18</v>
@@ -381,32 +382,32 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
@@ -415,29 +416,29 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>25</v>
@@ -446,49 +447,49 @@
         <v>6</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>30</v>
@@ -497,61 +498,44 @@
         <v>6</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="0">
-        <v>19</v>
-      </c>
-      <c r="B19" s="0" t="s">
         <v>35</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -561,7 +545,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -584,66 +568,86 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>43</v>
       </c>
     </row>
@@ -684,7 +688,7 @@
         <v>44</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0">
         <v>22</v>
@@ -703,7 +707,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
<tab> moves through textboxes only, not drop downs
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -45,13 +45,10 @@
     <t>12/1/2017</t>
   </si>
   <si>
-    <t>tabbing from text should move to next text, not the drop downs</t>
+    <t>down-arrow from last line of text should move into next text box</t>
   </si>
   <si>
     <t>Feature</t>
-  </si>
-  <si>
-    <t>down-arrow from last line of text should move into next text box</t>
   </si>
   <si>
     <t>when new task is created, default set its drop downs to the same values as the one above it</t>
@@ -133,12 +130,15 @@
     <t>Done</t>
   </si>
   <si>
+    <t>tabbing from text should move to next text, not the drop downs</t>
+  </si>
+  <si>
+    <t>3/3/2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">have some key command to end the current task
 and immediately open and edit a new task below it
 Ctrl-N (Next or New)</t>
-  </si>
-  <si>
-    <t>3/3/2018</t>
   </si>
   <si>
     <t xml:space="preserve">Have executable be named Tamarin.exe to match installation program name
@@ -225,7 +225,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -268,7 +268,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -285,7 +285,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -302,7 +302,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>12</v>
@@ -311,7 +311,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>8</v>
@@ -319,7 +319,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>13</v>
@@ -328,35 +328,35 @@
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -365,63 +365,63 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>24</v>
@@ -433,12 +433,12 @@
         <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>25</v>
@@ -450,15 +450,15 @@
         <v>10</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -467,15 +467,15 @@
         <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
@@ -484,32 +484,32 @@
         <v>10</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>6</v>
@@ -518,24 +518,7 @@
         <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="0">
-        <v>2</v>
-      </c>
-      <c r="B18" s="0" t="s">
         <v>34</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -545,7 +528,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -568,18 +551,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>10</v>
@@ -588,66 +571,86 @@
         <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
+        <v>1</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
         <v>3</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>43</v>
       </c>
     </row>
@@ -707,7 +710,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
navigate among textboxes with up/down arrows
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -45,13 +45,10 @@
     <t>12/1/2017</t>
   </si>
   <si>
-    <t>down-arrow from last line of text should move into next text box</t>
+    <t>when new task is created, default set its drop downs to the same values as the one above it</t>
   </si>
   <si>
     <t>Feature</t>
-  </si>
-  <si>
-    <t>when new task is created, default set its drop downs to the same values as the one above it</t>
   </si>
   <si>
     <t xml:space="preserve">deactivate mouse scroll when hovering over dropdowns
@@ -130,10 +127,14 @@
     <t>Done</t>
   </si>
   <si>
+    <t xml:space="preserve">down-arrow from last line of text should move into next text box
+and up-arrow should move to previous field</t>
+  </si>
+  <si>
+    <t>3/3/2018</t>
+  </si>
+  <si>
     <t>tabbing from text should move to next text, not the drop downs</t>
-  </si>
-  <si>
-    <t>3/3/2018</t>
   </si>
   <si>
     <t xml:space="preserve">have some key command to end the current task
@@ -225,7 +226,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -268,7 +269,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -285,7 +286,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -294,7 +295,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>8</v>
@@ -302,7 +303,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>12</v>
@@ -311,35 +312,35 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -348,63 +349,63 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>23</v>
@@ -416,12 +417,12 @@
         <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>24</v>
@@ -433,15 +434,15 @@
         <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -450,15 +451,15 @@
         <v>10</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -467,32 +468,32 @@
         <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>6</v>
@@ -501,24 +502,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="0">
-        <v>2</v>
-      </c>
-      <c r="B17" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -528,7 +512,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -551,18 +535,18 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>10</v>
@@ -571,18 +555,18 @@
         <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>10</v>
@@ -591,66 +575,86 @@
         <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
+        <v>1</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
         <v>3</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="D7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>43</v>
       </c>
     </row>
@@ -710,7 +714,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
disable mousewheel on comboboxes
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Id</t>
   </si>
@@ -29,6 +29,18 @@
   </si>
   <si>
     <t>Created</t>
+  </si>
+  <si>
+    <t>when combox value is changed, return focus to textbox</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>3/3/2018</t>
   </si>
   <si>
     <t xml:space="preserve">if category A is removed, and category B is added,
@@ -36,9 +48,6 @@
 then all category A tasks are auto reset to B - they should not be</t>
   </si>
   <si>
-    <t>Todo</t>
-  </si>
-  <si>
     <t>Bug</t>
   </si>
   <si>
@@ -46,19 +55,6 @@
   </si>
   <si>
     <t>when new task is created, default set its drop downs to the same values as the one above it</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deactivate mouse scroll when hovering over dropdowns
-i accidently set 5 rows to Done with one scroll</t>
-  </si>
-  <si>
-    <t>icon for program</t>
-  </si>
-  <si>
-    <t>12/5/2017</t>
   </si>
   <si>
     <t>when click + (add task) button, and new task is below scroll viewable area, should auto scoll to focus on new task</t>
@@ -127,11 +123,18 @@
     <t>Done</t>
   </si>
   <si>
+    <t>icon for program</t>
+  </si>
+  <si>
+    <t>12/5/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deactivate mouse scroll when hovering over dropdowns
+i accidently set 5 rows to Done with one scroll</t>
+  </si>
+  <si>
     <t xml:space="preserve">down-arrow from last line of text should move into next text box
 and up-arrow should move to previous field</t>
-  </si>
-  <si>
-    <t>3/3/2018</t>
   </si>
   <si>
     <t>tabbing from text should move to next text, not the drop downs</t>
@@ -226,7 +229,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -252,7 +255,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -269,7 +272,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -281,32 +284,32 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -315,32 +318,32 @@
         <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -349,15 +352,15 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -366,29 +369,29 @@
         <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>22</v>
@@ -397,15 +400,15 @@
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>23</v>
@@ -414,52 +417,52 @@
         <v>6</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>6</v>
@@ -468,41 +471,24 @@
         <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="0">
-        <v>2</v>
-      </c>
-      <c r="B16" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +498,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -535,127 +521,167 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
+        <v>21</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>1</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
         <v>3</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>43</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -676,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -684,7 +710,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
@@ -692,43 +718,43 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F2" s="0">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refocus on textbox when combobox changes
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -31,23 +31,14 @@
     <t>Created</t>
   </si>
   <si>
-    <t>when combox value is changed, return focus to textbox</t>
-  </si>
-  <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>3/3/2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">if category A is removed, and category B is added,
 and category A is a starting-sub-string of B
 then all category A tasks are auto reset to B - they should not be</t>
   </si>
   <si>
+    <t>Todo</t>
+  </si>
+  <si>
     <t>Bug</t>
   </si>
   <si>
@@ -55,6 +46,9 @@
   </si>
   <si>
     <t>when new task is created, default set its drop downs to the same values as the one above it</t>
+  </si>
+  <si>
+    <t>Feature</t>
   </si>
   <si>
     <t>when click + (add task) button, and new task is below scroll viewable area, should auto scoll to focus on new task</t>
@@ -121,6 +115,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>when combox value is changed, return focus to textbox</t>
+  </si>
+  <si>
+    <t>3/3/2018</t>
   </si>
   <si>
     <t>icon for program</t>
@@ -229,7 +229,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -255,7 +255,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -272,7 +272,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -284,29 +284,29 @@
         <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
@@ -315,7 +315,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>14</v>
@@ -323,7 +323,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>15</v>
@@ -340,7 +340,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>17</v>
@@ -357,7 +357,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>19</v>
@@ -369,46 +369,46 @@
         <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>23</v>
@@ -417,7 +417,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>24</v>
@@ -425,7 +425,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>25</v>
@@ -434,7 +434,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
         <v>26</v>
@@ -442,7 +442,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>27</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>29</v>
@@ -468,27 +468,10 @@
         <v>6</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="0">
-        <v>2</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -498,7 +481,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -521,166 +504,186 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>35</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="F8" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
+        <v>1</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
         <v>3</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B10" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="0" t="s">
+      <c r="C10" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="0" t="s">
         <v>44</v>
       </c>
     </row>
@@ -721,7 +724,7 @@
         <v>45</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0">
         <v>23</v>
@@ -740,13 +743,13 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>49</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">

</xml_diff>

<commit_message>
new task defaults status and category to the task above it
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -45,25 +45,22 @@
     <t>12/1/2017</t>
   </si>
   <si>
-    <t>when new task is created, default set its drop downs to the same values as the one above it</t>
+    <t>when click + (add task) button, and new task is below scroll viewable area, should auto scoll to focus on new task</t>
+  </si>
+  <si>
+    <t>12/7/2017</t>
+  </si>
+  <si>
+    <t>warn when closing with unsaved data</t>
+  </si>
+  <si>
+    <t>12/8/2017</t>
+  </si>
+  <si>
+    <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
   </si>
   <si>
     <t>Feature</t>
-  </si>
-  <si>
-    <t>when click + (add task) button, and new task is below scroll viewable area, should auto scoll to focus on new task</t>
-  </si>
-  <si>
-    <t>12/7/2017</t>
-  </si>
-  <si>
-    <t>warn when closing with unsaved data</t>
-  </si>
-  <si>
-    <t>12/8/2017</t>
-  </si>
-  <si>
-    <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
   </si>
   <si>
     <t>12/14/2017</t>
@@ -117,10 +114,13 @@
     <t>Done</t>
   </si>
   <si>
+    <t>when new task is created, default set its drop downs to the same values as the one above it</t>
+  </si>
+  <si>
+    <t>3/3/2018</t>
+  </si>
+  <si>
     <t>when combox value is changed, return focus to textbox</t>
-  </si>
-  <si>
-    <t>3/3/2018</t>
   </si>
   <si>
     <t>icon for program</t>
@@ -229,7 +229,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -272,7 +272,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -281,15 +281,15 @@
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -306,7 +306,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
@@ -315,49 +315,49 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>19</v>
@@ -366,15 +366,15 @@
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>20</v>
@@ -383,69 +383,69 @@
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -454,24 +454,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0">
-        <v>2</v>
-      </c>
-      <c r="B14" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -481,7 +464,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -504,186 +487,206 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
+        <v>1</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
         <v>3</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B11" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="0" t="s">
+      <c r="C11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="0" t="s">
         <v>44</v>
       </c>
     </row>
@@ -724,7 +727,7 @@
         <v>45</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0">
         <v>23</v>
@@ -743,7 +746,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
auto-scroll to keep focused textbox view
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -45,12 +45,6 @@
     <t>12/1/2017</t>
   </si>
   <si>
-    <t>when click + (add task) button, and new task is below scroll viewable area, should auto scoll to focus on new task</t>
-  </si>
-  <si>
-    <t>12/7/2017</t>
-  </si>
-  <si>
     <t>warn when closing with unsaved data</t>
   </si>
   <si>
@@ -114,10 +108,16 @@
     <t>Done</t>
   </si>
   <si>
+    <t>when click + (add task) button, and new task is below scroll viewable area, should auto scoll to focus on new task</t>
+  </si>
+  <si>
+    <t>12/7/2017</t>
+  </si>
+  <si>
+    <t>3/3/2018</t>
+  </si>
+  <si>
     <t>when new task is created, default set its drop downs to the same values as the one above it</t>
-  </si>
-  <si>
-    <t>3/3/2018</t>
   </si>
   <si>
     <t>when combox value is changed, return focus to textbox</t>
@@ -229,7 +229,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -272,7 +272,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -289,7 +289,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -298,24 +298,24 @@
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>15</v>
@@ -323,7 +323,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>16</v>
@@ -332,49 +332,49 @@
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
+        <v>16</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>20</v>
@@ -383,7 +383,7 @@
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>21</v>
@@ -391,7 +391,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>22</v>
@@ -400,7 +400,7 @@
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>23</v>
@@ -408,7 +408,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>24</v>
@@ -417,7 +417,7 @@
         <v>6</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>25</v>
@@ -425,7 +425,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>26</v>
@@ -438,23 +438,6 @@
       </c>
       <c r="E12" s="0" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0">
-        <v>2</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -464,7 +447,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -487,206 +470,226 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
+        <v>1</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
         <v>3</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B12" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="0" t="s">
+      <c r="C12" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>44</v>
       </c>
     </row>
@@ -727,7 +730,7 @@
         <v>45</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0">
         <v>23</v>
@@ -746,7 +749,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
minimize space between elements
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -71,50 +71,50 @@
     <t>only allow one instance of this program open at a time</t>
   </si>
   <si>
+    <t>option to clear inactive list</t>
+  </si>
+  <si>
+    <t>12/18/2017</t>
+  </si>
+  <si>
+    <t>if there are zero or one Category options total, then hide category column on both pages</t>
+  </si>
+  <si>
+    <t>1/7/2018</t>
+  </si>
+  <si>
+    <t>get the msi installed program to run again - it won't run</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
+  </si>
+  <si>
+    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
+  </si>
+  <si>
+    <t>10/28/2017</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>have as little border space between elements as possible</t>
+  </si>
+  <si>
+    <t>12/19/2017</t>
+  </si>
+  <si>
+    <t>3/3/2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">size text areas so no scrolling is ever needed
 - always apply scrolling to the whole pane, not to any of the inputs</t>
   </si>
   <si>
-    <t>option to clear inactive list</t>
-  </si>
-  <si>
-    <t>12/18/2017</t>
-  </si>
-  <si>
-    <t>have have as little border space between elements as possible</t>
-  </si>
-  <si>
-    <t>12/19/2017</t>
-  </si>
-  <si>
-    <t>if there are zero or one Category options total, then hide category column on both pages</t>
-  </si>
-  <si>
-    <t>1/7/2018</t>
-  </si>
-  <si>
-    <t>get the msi installed program to run again - it won't run</t>
-  </si>
-  <si>
-    <t>3/2/2018</t>
-  </si>
-  <si>
-    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
-  </si>
-  <si>
-    <t>10/28/2017</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>when click + (add task) button, and new task is below scroll viewable area, should auto scoll to focus on new task</t>
   </si>
   <si>
     <t>12/7/2017</t>
-  </si>
-  <si>
-    <t>3/3/2018</t>
   </si>
   <si>
     <t>when new task is created, default set its drop downs to the same values as the one above it</t>
@@ -229,7 +229,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -340,7 +340,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>17</v>
@@ -352,15 +352,15 @@
         <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -369,75 +369,41 @@
         <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0">
-        <v>22</v>
-      </c>
-      <c r="B11" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0">
-        <v>2</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -447,7 +413,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -470,158 +436,158 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>12</v>
@@ -630,66 +596,106 @@
         <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
+        <v>21</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>1</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
         <v>3</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B14" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="C14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>44</v>
       </c>
     </row>
@@ -749,7 +755,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
warn when closing with unsaved data
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Id</t>
   </si>
@@ -45,12 +45,6 @@
     <t>12/1/2017</t>
   </si>
   <si>
-    <t>warn when closing with unsaved data</t>
-  </si>
-  <si>
-    <t>12/8/2017</t>
-  </si>
-  <si>
     <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
   </si>
   <si>
@@ -96,6 +90,15 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>warn when closing with unsaved data</t>
+  </si>
+  <si>
+    <t>12/8/2017</t>
+  </si>
+  <si>
+    <t>3/5/2018</t>
   </si>
   <si>
     <t>have as little border space between elements as possible</t>
@@ -229,7 +232,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -272,7 +275,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -281,24 +284,24 @@
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>13</v>
@@ -306,7 +309,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>14</v>
@@ -315,32 +318,32 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
+        <v>17</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>17</v>
@@ -349,7 +352,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>18</v>
@@ -357,7 +360,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>19</v>
@@ -366,7 +369,7 @@
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>20</v>
@@ -374,7 +377,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>21</v>
@@ -387,23 +390,6 @@
       </c>
       <c r="E9" s="0" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0">
-        <v>2</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -413,7 +399,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -436,267 +422,287 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>30</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="F5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>8</v>
-      </c>
       <c r="F8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>41</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
+        <v>1</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
         <v>3</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="0" t="s">
+      <c r="B15" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -717,7 +723,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -725,7 +731,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2">
@@ -733,10 +739,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="0">
         <v>23</v>
@@ -744,21 +750,21 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
@@ -766,10 +772,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
notify if file edited by outside source; option to reload
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -54,51 +54,51 @@
     <t>12/14/2017</t>
   </si>
   <si>
+    <t>only allow one instance of this program open at a time</t>
+  </si>
+  <si>
+    <t>12/15/2017</t>
+  </si>
+  <si>
+    <t>option to clear inactive list</t>
+  </si>
+  <si>
+    <t>12/18/2017</t>
+  </si>
+  <si>
+    <t>if there are zero or one Category options total, then hide category column on both pages</t>
+  </si>
+  <si>
+    <t>1/7/2018</t>
+  </si>
+  <si>
+    <t>get the msi installed program to run again - it won't run</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
+  </si>
+  <si>
+    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
+  </si>
+  <si>
+    <t>10/28/2017</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t xml:space="preserve">notify if file was changed by another program
 - or another instance of this program
 - reload or overwrite</t>
   </si>
   <si>
-    <t>12/15/2017</t>
-  </si>
-  <si>
-    <t>only allow one instance of this program open at a time</t>
-  </si>
-  <si>
-    <t>option to clear inactive list</t>
-  </si>
-  <si>
-    <t>12/18/2017</t>
-  </si>
-  <si>
-    <t>if there are zero or one Category options total, then hide category column on both pages</t>
-  </si>
-  <si>
-    <t>1/7/2018</t>
-  </si>
-  <si>
-    <t>get the msi installed program to run again - it won't run</t>
-  </si>
-  <si>
-    <t>3/2/2018</t>
-  </si>
-  <si>
-    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
-  </si>
-  <si>
-    <t>10/28/2017</t>
-  </si>
-  <si>
-    <t>Done</t>
+    <t>3/5/2018</t>
   </si>
   <si>
     <t>warn when closing with unsaved data</t>
   </si>
   <si>
     <t>12/8/2017</t>
-  </si>
-  <si>
-    <t>3/5/2018</t>
   </si>
   <si>
     <t>have as little border space between elements as possible</t>
@@ -232,7 +232,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -292,7 +292,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>12</v>
@@ -301,7 +301,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>13</v>
@@ -309,7 +309,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>14</v>
@@ -321,49 +321,49 @@
         <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
+        <v>22</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -372,24 +372,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0">
-        <v>2</v>
-      </c>
-      <c r="B9" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -399,7 +382,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -422,64 +405,64 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>29</v>
@@ -487,19 +470,19 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>29</v>
@@ -507,19 +490,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>29</v>
@@ -527,19 +510,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>29</v>
@@ -547,19 +530,19 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>29</v>
@@ -567,19 +550,19 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>29</v>
@@ -587,16 +570,16 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>8</v>
@@ -607,13 +590,13 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>10</v>
@@ -627,13 +610,13 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>10</v>
@@ -647,19 +630,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>29</v>
@@ -667,41 +650,61 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
+        <v>1</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0">
         <v>3</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B16" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="0" t="s">
+      <c r="C16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="0" t="s">
         <v>45</v>
       </c>
     </row>
@@ -761,7 +764,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
bug fix: checking unnamed files for outside edits
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -232,7 +232,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -292,10 +292,10 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>6</v>
@@ -304,15 +304,15 @@
         <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>6</v>
@@ -321,32 +321,32 @@
         <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -355,23 +355,6 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0">
-        <v>2</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="0" t="s">
         <v>21</v>
       </c>
     </row>
@@ -382,7 +365,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,16 +393,16 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>13</v>
@@ -430,10 +413,10 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>22</v>
@@ -442,7 +425,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>24</v>
@@ -450,30 +433,30 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>22</v>
@@ -482,7 +465,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>29</v>
@@ -490,19 +473,19 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>29</v>
@@ -510,19 +493,19 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>29</v>
@@ -530,10 +513,10 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>22</v>
@@ -542,7 +525,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>29</v>
@@ -550,10 +533,10 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>22</v>
@@ -562,7 +545,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>29</v>
@@ -570,19 +553,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>29</v>
@@ -590,16 +573,16 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
         <v>8</v>
@@ -610,10 +593,10 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>22</v>
@@ -630,10 +613,10 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>22</v>
@@ -650,10 +633,10 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>22</v>
@@ -662,7 +645,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>29</v>
@@ -670,41 +653,61 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>22</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
+        <v>1</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0">
         <v>3</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B17" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="C17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F17" s="0" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
select first tab when opening multiple
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>Id</t>
   </si>
@@ -45,57 +45,76 @@
     <t>12/1/2017</t>
   </si>
   <si>
+    <t>enter in row number field should accept the edit</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>4/10/2018</t>
+  </si>
+  <si>
+    <t>option to clear inactive list</t>
+  </si>
+  <si>
+    <t>12/18/2017</t>
+  </si>
+  <si>
+    <t>get the msi installed program to run again - it won't run</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
+  </si>
+  <si>
+    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
+  </si>
+  <si>
+    <t>10/28/2017</t>
+  </si>
+  <si>
+    <t>editing statuses or categories does not prompt a Save when you close</t>
+  </si>
+  <si>
+    <t>4/11/2018</t>
+  </si>
+  <si>
+    <t>when moving a row, move cursor to the row that is now in the position that the moved row previously held</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think fixing the lingering layout/scrolling issues will require a massive redesign of the gui layout system
+maybe in version 3</t>
+  </si>
+  <si>
+    <t>visual indication that a list has been edited but not saved</t>
+  </si>
+  <si>
     <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
   </si>
   <si>
-    <t>Feature</t>
-  </si>
-  <si>
     <t>12/14/2017</t>
   </si>
   <si>
-    <t>option to clear inactive list</t>
-  </si>
-  <si>
-    <t>12/18/2017</t>
+    <t>you can move a row to a row higher than you should be able to</t>
+  </si>
+  <si>
+    <t>adding a task with Add Button does not set task height properly</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>on Load Previous Projects - auto select first project in list instead of last</t>
   </si>
   <si>
     <t>if there are zero or one Category options total, then hide category column on both pages</t>
   </si>
   <si>
     <t>1/7/2018</t>
-  </si>
-  <si>
-    <t>get the msi installed program to run again - it won't run</t>
-  </si>
-  <si>
-    <t>3/2/2018</t>
-  </si>
-  <si>
-    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
-  </si>
-  <si>
-    <t>10/28/2017</t>
-  </si>
-  <si>
-    <t>enter in row number field should accept the edit</t>
-  </si>
-  <si>
-    <t>4/10/2018</t>
-  </si>
-  <si>
-    <t>on Load Previous Projects - auto select first project in list instead of last</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t xml:space="preserve">changing between active and inactive - need a reminder to the program to update titleBox sizes
 and UpdateTextBoxSizes does not help - UPDATE now it does
 only affects some titles</t>
-  </si>
-  <si>
-    <t>4/11/2018</t>
   </si>
   <si>
     <t xml:space="preserve">the scroll bar is way way longer than the content
@@ -260,7 +279,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -303,7 +322,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -337,7 +356,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>14</v>
@@ -346,7 +365,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>15</v>
@@ -354,7 +373,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>16</v>
@@ -371,7 +390,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>18</v>
@@ -380,7 +399,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
         <v>19</v>
@@ -388,7 +407,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>20</v>
@@ -397,27 +416,95 @@
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>34</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>21</v>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>13</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>30</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>31</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -427,7 +514,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -450,141 +537,141 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>36</v>
@@ -595,19 +682,19 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>37</v>
@@ -615,153 +702,153 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>10</v>
@@ -770,67 +857,107 @@
         <v>8</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>51</v>
+        <v>8</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
+        <v>21</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="0">
+        <v>1</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="0">
         <v>3</v>
       </c>
-      <c r="B20" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>53</v>
+      <c r="B22" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -851,7 +978,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -859,7 +986,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2">
@@ -867,32 +994,32 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="0">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
@@ -900,10 +1027,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
option to clear inactive list
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -54,12 +54,6 @@
     <t>4/10/2018</t>
   </si>
   <si>
-    <t>option to clear inactive list</t>
-  </si>
-  <si>
-    <t>12/18/2017</t>
-  </si>
-  <si>
     <t>get the msi installed program to run again - it won't run</t>
   </si>
   <si>
@@ -101,6 +95,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>option to clear inactive list</t>
+  </si>
+  <si>
+    <t>12/18/2017</t>
   </si>
   <si>
     <t>on Load Previous Projects - auto select first project in list instead of last</t>
@@ -279,7 +279,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -339,7 +339,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>12</v>
@@ -348,7 +348,7 @@
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>13</v>
@@ -356,7 +356,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>14</v>
@@ -373,7 +373,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>16</v>
@@ -382,7 +382,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E6" s="0" t="s">
         <v>17</v>
@@ -390,7 +390,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>18</v>
@@ -399,18 +399,18 @@
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
@@ -419,46 +419,46 @@
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0">
-        <v>34</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>23</v>
@@ -467,18 +467,18 @@
         <v>6</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>6</v>
@@ -487,24 +487,7 @@
         <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="0">
-        <v>31</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -514,7 +497,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -537,78 +520,78 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
@@ -617,18 +600,18 @@
         <v>11</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>7</v>
@@ -637,41 +620,41 @@
         <v>11</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E8" s="0" t="s">
         <v>36</v>
@@ -682,19 +665,19 @@
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>37</v>
@@ -702,39 +685,39 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>43</v>
@@ -742,19 +725,19 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>43</v>
@@ -762,19 +745,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>43</v>
@@ -782,19 +765,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>43</v>
@@ -802,19 +785,19 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>43</v>
@@ -822,19 +805,19 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>43</v>
@@ -842,16 +825,16 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
         <v>8</v>
@@ -862,13 +845,13 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>10</v>
@@ -882,13 +865,13 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>10</v>
@@ -902,19 +885,19 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>43</v>
@@ -922,41 +905,61 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
+        <v>1</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0">
         <v>3</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B23" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="0" t="s">
+      <c r="C23" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1016,7 +1019,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
press enter to move row
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -31,48 +31,42 @@
     <t>Created</t>
   </si>
   <si>
+    <t>when moving a row, move cursor to the row that is now in the position that the moved row previously held</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>4/11/2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">if category A is removed, and category B is added,
 and category A is a starting-sub-string of B
 then all category A tasks are auto reset to B - they should not be</t>
   </si>
   <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
     <t>12/1/2017</t>
   </si>
   <si>
-    <t>enter in row number field should accept the edit</t>
+    <t>get the msi installed program to run again - it won't run</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
+  </si>
+  <si>
+    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
+  </si>
+  <si>
+    <t>10/28/2017</t>
+  </si>
+  <si>
+    <t>editing statuses or categories does not prompt a Save when you close</t>
   </si>
   <si>
     <t>Feature</t>
-  </si>
-  <si>
-    <t>4/10/2018</t>
-  </si>
-  <si>
-    <t>get the msi installed program to run again - it won't run</t>
-  </si>
-  <si>
-    <t>3/2/2018</t>
-  </si>
-  <si>
-    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
-  </si>
-  <si>
-    <t>10/28/2017</t>
-  </si>
-  <si>
-    <t>editing statuses or categories does not prompt a Save when you close</t>
-  </si>
-  <si>
-    <t>4/11/2018</t>
-  </si>
-  <si>
-    <t>when moving a row, move cursor to the row that is now in the position that the moved row previously held</t>
   </si>
   <si>
     <t xml:space="preserve">I think fixing the lingering layout/scrolling issues will require a massive redesign of the gui layout system
@@ -95,6 +89,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>enter in row number field should accept the edit</t>
+  </si>
+  <si>
+    <t>4/10/2018</t>
   </si>
   <si>
     <t>option to clear inactive list</t>
@@ -279,7 +279,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -305,7 +305,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -322,7 +322,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -331,10 +331,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -342,16 +342,16 @@
         <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>12</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5">
@@ -359,16 +359,16 @@
         <v>2</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6">
@@ -376,24 +376,24 @@
         <v>29</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
@@ -402,46 +402,46 @@
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="0">
-        <v>34</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>21</v>
@@ -450,18 +450,18 @@
         <v>6</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>6</v>
@@ -470,24 +470,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="0">
-        <v>31</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -497,7 +480,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -520,161 +503,161 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>27</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="F6" s="0" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
+        <v>24</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>36</v>
@@ -685,19 +668,19 @@
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>37</v>
@@ -705,39 +688,39 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>43</v>
@@ -745,19 +728,19 @@
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>43</v>
@@ -765,19 +748,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>43</v>
@@ -785,19 +768,19 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>43</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>43</v>
@@ -805,19 +788,19 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>43</v>
@@ -825,19 +808,19 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>43</v>
@@ -845,19 +828,19 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>43</v>
@@ -865,19 +848,19 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D19" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>43</v>
@@ -885,19 +868,19 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>43</v>
@@ -905,19 +888,19 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>43</v>
@@ -925,41 +908,61 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
+        <v>1</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0">
         <v>3</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B24" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="0" t="s">
+      <c r="C24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1000,7 +1003,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0">
         <v>34</v>
@@ -1019,7 +1022,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
cursor position when moving between rows
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -31,23 +31,17 @@
     <t>Created</t>
   </si>
   <si>
-    <t>when moving a row, move cursor to the row that is now in the position that the moved row previously held</t>
-  </si>
-  <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
-    <t>4/11/2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">if category A is removed, and category B is added,
 and category A is a starting-sub-string of B
 then all category A tasks are auto reset to B - they should not be</t>
   </si>
   <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
     <t>12/1/2017</t>
   </si>
   <si>
@@ -67,6 +61,9 @@
   </si>
   <si>
     <t>Feature</t>
+  </si>
+  <si>
+    <t>4/11/2018</t>
   </si>
   <si>
     <t xml:space="preserve">I think fixing the lingering layout/scrolling issues will require a massive redesign of the gui layout system
@@ -89,6 +86,9 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>when moving a row, move cursor to the row that is now in the position that the moved row previously held</t>
   </si>
   <si>
     <t>enter in row number field should accept the edit</t>
@@ -279,7 +279,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -305,7 +305,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -322,7 +322,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -339,7 +339,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -356,7 +356,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
@@ -365,32 +365,32 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>17</v>
@@ -399,49 +399,49 @@
         <v>6</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="0">
-        <v>34</v>
-      </c>
-      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>13</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>8</v>
+      <c r="D9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>21</v>
@@ -453,24 +453,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="0">
-        <v>31</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -480,7 +463,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -503,118 +486,118 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
@@ -623,18 +606,18 @@
         <v>25</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
@@ -643,41 +626,41 @@
         <v>25</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E10" s="0" t="s">
         <v>36</v>
@@ -688,19 +671,19 @@
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>37</v>
@@ -708,39 +691,39 @@
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>43</v>
@@ -748,19 +731,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>43</v>
@@ -768,19 +751,19 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>43</v>
@@ -788,19 +771,19 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>43</v>
@@ -808,19 +791,19 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>43</v>
@@ -828,19 +811,19 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>43</v>
@@ -848,19 +831,19 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>43</v>
@@ -868,19 +851,19 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>43</v>
@@ -888,19 +871,19 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>43</v>
@@ -908,19 +891,19 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>43</v>
@@ -928,41 +911,61 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
+        <v>1</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0">
         <v>3</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B25" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="0" t="s">
+      <c r="C25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1003,7 +1006,7 @@
         <v>60</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0">
         <v>34</v>
@@ -1022,7 +1025,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
edit status or categories prompts saving
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Id</t>
   </si>
@@ -57,22 +57,19 @@
     <t>10/28/2017</t>
   </si>
   <si>
-    <t>editing statuses or categories does not prompt a Save when you close</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>4/11/2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">I think fixing the lingering layout/scrolling issues will require a massive redesign of the gui layout system
 maybe in version 3</t>
   </si>
   <si>
+    <t>4/11/2018</t>
+  </si>
+  <si>
     <t>visual indication that a list has been edited but not saved</t>
   </si>
   <si>
+    <t>Feature</t>
+  </si>
+  <si>
     <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
   </si>
   <si>
@@ -86,6 +83,12 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>editing statuses or categories does not prompt a Save when you close</t>
+  </si>
+  <si>
+    <t>ctrl-up/down arrow to jump from task to task, instead of through the lines of a task</t>
   </si>
   <si>
     <t>when moving a row, move cursor to the row that is now in the position that the moved row previously held</t>
@@ -279,7 +282,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -356,7 +359,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
@@ -365,66 +368,66 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="0">
-        <v>34</v>
-      </c>
-      <c r="B7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>13</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>15</v>
+      <c r="D8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>20</v>
@@ -436,24 +439,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="0">
-        <v>31</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -463,7 +449,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -486,487 +472,527 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E21" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E22" s="0" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>57</v>
+        <v>8</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0">
+        <v>21</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0">
+        <v>1</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0">
         <v>3</v>
       </c>
-      <c r="B25" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="B27" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="0" t="s">
-        <v>59</v>
+      <c r="F27" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -987,7 +1013,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -995,7 +1021,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2">
@@ -1003,32 +1029,32 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
@@ -1036,10 +1062,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fix: combo box matching on prefix-string
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -31,58 +31,58 @@
     <t>Created</t>
   </si>
   <si>
+    <t>get the msi installed program to run again - it won't run</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
+  </si>
+  <si>
+    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
+  </si>
+  <si>
+    <t>10/28/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I think fixing the lingering layout/scrolling issues will require a massive redesign of the gui layout system
+maybe in version 3</t>
+  </si>
+  <si>
+    <t>4/11/2018</t>
+  </si>
+  <si>
+    <t>visual indication that a list has been edited but not saved</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
+  </si>
+  <si>
+    <t>12/14/2017</t>
+  </si>
+  <si>
+    <t>you can move a row to a row higher than you should be able to</t>
+  </si>
+  <si>
+    <t>adding a task with Add Button does not set task height properly</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
     <t xml:space="preserve">if category A is removed, and category B is added,
 and category A is a starting-sub-string of B
 then all category A tasks are auto reset to B - they should not be</t>
   </si>
   <si>
-    <t>Todo</t>
-  </si>
-  <si>
-    <t>Bug</t>
-  </si>
-  <si>
     <t>12/1/2017</t>
-  </si>
-  <si>
-    <t>get the msi installed program to run again - it won't run</t>
-  </si>
-  <si>
-    <t>3/2/2018</t>
-  </si>
-  <si>
-    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
-  </si>
-  <si>
-    <t>10/28/2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I think fixing the lingering layout/scrolling issues will require a massive redesign of the gui layout system
-maybe in version 3</t>
-  </si>
-  <si>
-    <t>4/11/2018</t>
-  </si>
-  <si>
-    <t>visual indication that a list has been edited but not saved</t>
-  </si>
-  <si>
-    <t>Feature</t>
-  </si>
-  <si>
-    <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
-  </si>
-  <si>
-    <t>12/14/2017</t>
-  </si>
-  <si>
-    <t>you can move a row to a row higher than you should be able to</t>
-  </si>
-  <si>
-    <t>adding a task with Add Button does not set task height properly</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>editing statuses or categories does not prompt a Save when you close</t>
@@ -282,7 +282,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -308,7 +308,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>5</v>
@@ -325,7 +325,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -342,7 +342,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -359,7 +359,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
@@ -368,32 +368,32 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0">
-        <v>34</v>
-      </c>
-      <c r="B6" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>17</v>
@@ -402,18 +402,18 @@
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -422,24 +422,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0">
-        <v>31</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -449,7 +432,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -472,178 +455,178 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
+        <v>17</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>26</v>
-      </c>
       <c r="F7" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
@@ -652,18 +635,18 @@
         <v>26</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
@@ -672,41 +655,41 @@
         <v>26</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E13" s="0" t="s">
         <v>37</v>
@@ -717,19 +700,19 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>38</v>
@@ -737,39 +720,39 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>44</v>
@@ -777,19 +760,19 @@
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>44</v>
@@ -797,19 +780,19 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>44</v>
@@ -817,19 +800,19 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C19" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>44</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>44</v>
@@ -837,19 +820,19 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>44</v>
@@ -857,19 +840,19 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>44</v>
@@ -877,19 +860,19 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>44</v>
@@ -897,19 +880,19 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>44</v>
@@ -917,19 +900,19 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="D24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>8</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>44</v>
@@ -937,19 +920,19 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
+        <v>4</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>10</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>44</v>
@@ -957,41 +940,61 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
+        <v>1</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0">
         <v>3</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B28" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" s="0" t="s">
+      <c r="C28" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1032,7 +1035,7 @@
         <v>61</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0">
         <v>37</v>
@@ -1051,7 +1054,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
installer will add shortcut on desktop
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Id</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Feature</t>
+  </si>
+  <si>
+    <t>better icon</t>
   </si>
   <si>
     <t>make it more obvious which tab is selected - with color or by removing the border between tab and pane</t>
@@ -230,6 +233,9 @@
   </si>
   <si>
     <t>Inactive</t>
+  </si>
+  <si>
+    <t>get the msi installed program to run again - it won't run after installation</t>
   </si>
 </sst>
 </file>
@@ -282,7 +288,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -311,7 +317,7 @@
         <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -374,43 +380,43 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0">
-        <v>13</v>
-      </c>
-      <c r="B7" s="0" t="s">
+    <row r="6">
+      <c r="A6" s="0">
+        <v>38</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>16</v>
+      <c r="D6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>18</v>
@@ -422,6 +428,23 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>31</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>12</v>
       </c>
     </row>
@@ -455,7 +478,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2">
@@ -463,16 +486,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F2" s="0" t="s">
         <v>12</v>
@@ -483,10 +506,10 @@
         <v>29</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>14</v>
@@ -503,10 +526,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
@@ -523,10 +546,10 @@
         <v>32</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
@@ -543,16 +566,16 @@
         <v>26</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>12</v>
@@ -563,16 +586,16 @@
         <v>17</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>12</v>
@@ -583,16 +606,16 @@
         <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>12</v>
@@ -603,16 +626,16 @@
         <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>12</v>
@@ -623,16 +646,16 @@
         <v>27</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>12</v>
@@ -643,16 +666,16 @@
         <v>24</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>12</v>
@@ -663,19 +686,19 @@
         <v>25</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13">
@@ -683,19 +706,19 @@
         <v>15</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14">
@@ -703,19 +726,19 @@
         <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15">
@@ -723,19 +746,19 @@
         <v>12</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16">
@@ -743,19 +766,19 @@
         <v>18</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17">
@@ -763,19 +786,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="0" t="s">
         <v>45</v>
-      </c>
-      <c r="C17" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18">
@@ -783,19 +806,19 @@
         <v>11</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19">
@@ -803,19 +826,19 @@
         <v>8</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20">
@@ -823,19 +846,19 @@
         <v>23</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21">
@@ -843,19 +866,19 @@
         <v>10</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22">
@@ -863,19 +886,19 @@
         <v>9</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23">
@@ -883,19 +906,19 @@
         <v>7</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24">
@@ -903,19 +926,19 @@
         <v>6</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25">
@@ -923,19 +946,19 @@
         <v>4</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26">
@@ -943,10 +966,10 @@
         <v>21</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>14</v>
@@ -955,7 +978,7 @@
         <v>8</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27">
@@ -963,16 +986,16 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F27" s="0" t="s">
         <v>8</v>
@@ -983,10 +1006,10 @@
         <v>3</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>14</v>
@@ -995,7 +1018,7 @@
         <v>10</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1016,7 +1039,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="s">
@@ -1024,7 +1047,7 @@
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -1032,32 +1055,32 @@
         <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>7</v>
@@ -1065,10 +1088,10 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
form icon as resource
</commit_message>
<xml_diff>
--- a/tmx_todo.xlsx
+++ b/tmx_todo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>Id</t>
   </si>
@@ -31,19 +31,13 @@
     <t>Created</t>
   </si>
   <si>
-    <t>get the msi installed program to run again - it won't run</t>
+    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
   </si>
   <si>
     <t>Todo</t>
   </si>
   <si>
     <t>Bug</t>
-  </si>
-  <si>
-    <t>3/2/2018</t>
-  </si>
-  <si>
-    <t>when first switching to pre-loaded tab, pause layout until visuals are ready</t>
   </si>
   <si>
     <t>10/28/2017</t>
@@ -78,6 +72,16 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">get the msi installed program to run again - it won't run after installation
+UPDATE
+the problem was that I manually set the WindowsForm icon file in the code and the file could not be found
+took that out since I set the icon file through project properties
+runs fine now</t>
+  </si>
+  <si>
+    <t>3/2/2018</t>
   </si>
   <si>
     <t xml:space="preserve">if category A is removed, and category B is added,
@@ -233,9 +237,6 @@
   </si>
   <si>
     <t>Inactive</t>
-  </si>
-  <si>
-    <t>get the msi installed program to run again - it won't run after installation</t>
   </si>
 </sst>
 </file>
@@ -288,7 +289,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -314,10 +315,10 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>6</v>
@@ -331,7 +332,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
@@ -348,7 +349,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
@@ -357,15 +358,15 @@
         <v>6</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>13</v>
@@ -374,32 +375,32 @@
         <v>6</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>13</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="0">
-        <v>38</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="C7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>16</v>
@@ -408,18 +409,18 @@
         <v>6</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>6</v>
@@ -428,24 +429,7 @@
         <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="0">
-        <v>31</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -455,7 +439,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -478,198 +462,198 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="F2" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
+        <v>17</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>30</v>
-      </c>
       <c r="C8" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>7</v>
@@ -678,18 +662,18 @@
         <v>27</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>7</v>
@@ -698,41 +682,41 @@
         <v>27</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
         <v>38</v>
@@ -743,19 +727,19 @@
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>39</v>
@@ -763,39 +747,39 @@
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>45</v>
@@ -803,19 +787,19 @@
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>45</v>
@@ -823,19 +807,19 @@
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>45</v>
@@ -843,19 +827,19 @@
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>45</v>
@@ -863,19 +847,19 @@
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>45</v>
@@ -883,19 +867,19 @@
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>45</v>
@@ -903,16 +887,16 @@
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>22</v>
@@ -923,16 +907,16 @@
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>22</v>
@@ -943,16 +927,16 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E25" s="0" t="s">
         <v>22</v>
@@ -963,19 +947,19 @@
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>45</v>
@@ -983,41 +967,61 @@
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C27" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>59</v>
-      </c>
       <c r="F27" s="0" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
+        <v>1</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="0">
         <v>3</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B29" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" s="0" t="s">
+      <c r="C29" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1058,7 +1062,7 @@
         <v>62</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2" s="0">
         <v>38</v>
@@ -1077,7 +1081,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>66</v>

</xml_diff>